<commit_message>
HW_02: new report done
</commit_message>
<xml_diff>
--- a/files/report_h2.xlsx
+++ b/files/report_h2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a17636999/Desktop/otus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a17636999/Projects/social-network/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="460" windowWidth="32560" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -266,7 +266,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -303,16 +303,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.82</c:v>
+                  <c:v>2.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.26</c:v>
+                  <c:v>5.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.67</c:v>
+                  <c:v>71.27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>398.26</c:v>
+                  <c:v>552.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,11 +328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1228542656"/>
-        <c:axId val="-1228048384"/>
+        <c:axId val="-1880177120"/>
+        <c:axId val="-1861625088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1228542656"/>
+        <c:axId val="-1880177120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +375,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1228048384"/>
+        <c:crossAx val="-1861625088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -383,7 +383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1228048384"/>
+        <c:axId val="-1861625088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,12 +433,14 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1228542656"/>
+        <c:crossAx val="-1880177120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -555,7 +557,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.441419871059807"/>
+          <c:y val="0.0202020202020202"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -608,76 +617,6 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$A$6:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$D$6:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.66</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.39</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Req/Sec after</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
@@ -710,21 +649,91 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>Лист1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Req/Sec after</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Лист1!$E$6:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>685.39</c:v>
+                  <c:v>512.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1914.35</c:v>
+                  <c:v>1345.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1856.48</c:v>
+                  <c:v>1353.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1957.53</c:v>
+                  <c:v>1512.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,11 +749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1191991536"/>
-        <c:axId val="-1191618576"/>
+        <c:axId val="-1859533472"/>
+        <c:axId val="-1859530720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1191991536"/>
+        <c:axId val="-1859533472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -787,7 +796,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1191618576"/>
+        <c:crossAx val="-1859530720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -795,7 +804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1191618576"/>
+        <c:axId val="-1859530720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +854,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1191991536"/>
+        <c:crossAx val="-1859533472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2045,13 +2054,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1250950</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>104201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>205801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2072,16 +2081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2368,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="166" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2407,13 +2416,13 @@
         <v>1250</v>
       </c>
       <c r="C6" s="2">
-        <v>1.82</v>
+        <v>2.39</v>
       </c>
       <c r="D6" s="1">
         <v>0.8</v>
       </c>
       <c r="E6" s="1">
-        <v>685.39</v>
+        <v>512.66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2424,13 +2433,13 @@
         <v>5390</v>
       </c>
       <c r="C7" s="2">
-        <v>3.26</v>
+        <v>5.76</v>
       </c>
       <c r="D7" s="1">
         <v>1.66</v>
       </c>
       <c r="E7" s="1">
-        <v>1914.35</v>
+        <v>1345.75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2441,13 +2450,13 @@
         <v>19580</v>
       </c>
       <c r="C8" s="2">
-        <v>51.67</v>
+        <v>71.27</v>
       </c>
       <c r="D8" s="1">
         <v>2.39</v>
       </c>
       <c r="E8" s="1">
-        <v>1856.48</v>
+        <v>1353.75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2458,13 +2467,13 @@
         <v>27420</v>
       </c>
       <c r="C9" s="2">
-        <v>398.26</v>
+        <v>552.39</v>
       </c>
       <c r="D9" s="1">
         <v>0.56000000000000005</v>
       </c>
       <c r="E9" s="1">
-        <v>1957.53</v>
+        <v>1512.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>